<commit_message>
#159 files for product csv upload
</commit_message>
<xml_diff>
--- a/public/misc/CSV_Upload.xlsx
+++ b/public/misc/CSV_Upload.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
   <si>
     <t>Number</t>
   </si>
@@ -64,15 +64,9 @@
     <t>Option Price</t>
   </si>
   <si>
-    <t>Option Image</t>
-  </si>
-  <si>
     <t>#111</t>
   </si>
   <si>
-    <t>Sample</t>
-  </si>
-  <si>
     <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit, sed do eiusmod tempor incididunt ut labore et dolore magna aliqua. Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut aliquip ex ea commodo consequat. Duis aute irure dolor in reprehenderit in voluptate velit esse cillum dolore eu fugiat nulla pariatur. Excepteur sint occaecat cupidatat non proident, sunt in culpa qui officia deserunt mollit anim id est laborum."</t>
   </si>
   <si>
@@ -85,31 +79,49 @@
     <t>Iphone</t>
   </si>
   <si>
-    <t>Electronics</t>
-  </si>
-  <si>
-    <t>Samsung</t>
-  </si>
-  <si>
-    <t>easyshop</t>
-  </si>
-  <si>
-    <t>product.jpeg</t>
-  </si>
-  <si>
     <t>Color</t>
   </si>
   <si>
     <t>Red</t>
   </si>
   <si>
-    <t>foorbar.jpg</t>
-  </si>
-  <si>
-    <t>product2.jpeg</t>
-  </si>
-  <si>
-    <t>Green</t>
+    <t>#222</t>
+  </si>
+  <si>
+    <t>Electronics &amp; Gadgets</t>
+  </si>
+  <si>
+    <t>Jewellery &amp; Watches</t>
+  </si>
+  <si>
+    <t>Sahara</t>
+  </si>
+  <si>
+    <t>Sanrio</t>
+  </si>
+  <si>
+    <t>partner1</t>
+  </si>
+  <si>
+    <t>partner2</t>
+  </si>
+  <si>
+    <t>Style</t>
+  </si>
+  <si>
+    <t>Slug</t>
+  </si>
+  <si>
+    <t>sample1</t>
+  </si>
+  <si>
+    <t>sample2</t>
+  </si>
+  <si>
+    <t>2.jpg</t>
+  </si>
+  <si>
+    <t>1.png</t>
   </si>
 </sst>
 </file>
@@ -442,10 +454,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="S1" sqref="S1:S3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -456,15 +468,16 @@
     <col min="4" max="5" width="11.5703125"/>
     <col min="6" max="6" width="7.28515625"/>
     <col min="7" max="7" width="17.140625"/>
-    <col min="8" max="10" width="11.5703125"/>
-    <col min="11" max="11" width="16.42578125"/>
-    <col min="12" max="12" width="17.85546875"/>
-    <col min="13" max="13" width="18.140625"/>
-    <col min="14" max="14" width="14.85546875"/>
-    <col min="15" max="1025" width="11.5703125"/>
+    <col min="8" max="8" width="11.5703125"/>
+    <col min="10" max="11" width="11.5703125"/>
+    <col min="12" max="12" width="16.42578125"/>
+    <col min="14" max="14" width="17.85546875"/>
+    <col min="15" max="15" width="18.140625"/>
+    <col min="16" max="16" width="14.85546875"/>
+    <col min="17" max="1027" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:18">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -490,101 +503,146 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+    </row>
+    <row r="2" spans="1:18">
+      <c r="A2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:17">
-      <c r="A2" t="s">
+      <c r="B2">
+        <v>11111</v>
+      </c>
+      <c r="C2" t="s">
         <v>17</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>18</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>19</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>20</v>
-      </c>
-      <c r="E2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" t="s">
-        <v>22</v>
       </c>
       <c r="G2">
         <v>32000</v>
       </c>
       <c r="H2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2">
+        <v>12</v>
+      </c>
+      <c r="M2" t="s">
+        <v>32</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2" t="s">
+        <v>35</v>
+      </c>
+      <c r="P2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R2">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
+      <c r="A3" t="s">
         <v>23</v>
       </c>
-      <c r="I2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="B3">
+        <v>22222</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3">
+        <v>32000</v>
+      </c>
+      <c r="H3" t="s">
         <v>25</v>
       </c>
-      <c r="K2">
+      <c r="I3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" t="s">
+        <v>29</v>
+      </c>
+      <c r="L3">
         <v>12</v>
       </c>
-      <c r="L2">
+      <c r="M3" t="s">
+        <v>33</v>
+      </c>
+      <c r="N3">
         <v>1</v>
       </c>
-      <c r="M2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N2" t="s">
-        <v>27</v>
-      </c>
-      <c r="O2" t="s">
-        <v>28</v>
-      </c>
-      <c r="P2">
+      <c r="O3" t="s">
+        <v>34</v>
+      </c>
+      <c r="P3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>22</v>
+      </c>
+      <c r="R3">
         <v>1200</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17">
-      <c r="M3" t="s">
-        <v>30</v>
-      </c>
-      <c r="N3" t="s">
-        <v>27</v>
-      </c>
-      <c r="O3" t="s">
-        <v>31</v>
-      </c>
-      <c r="P3">
-        <v>1200</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#159 changed excel formattings, applied dropdowns
</commit_message>
<xml_diff>
--- a/public/misc/CSV_Upload.xlsx
+++ b/public/misc/CSV_Upload.xlsx
@@ -4,17 +4,25 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="198"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="473" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Products" sheetId="1" r:id="rId1"/>
+    <sheet name="Attributes" sheetId="2" r:id="rId2"/>
+    <sheet name="Shipment" sheetId="8" r:id="rId3"/>
+    <sheet name="Locations" sheetId="7" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="location">#REF!,#REF!,#REF!,#REF!,#REF!</definedName>
+    <definedName name="locations">Locations!$A:$A</definedName>
+    <definedName name="shipping_locs">#REF!</definedName>
+  </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
   <si>
     <t>Number</t>
   </si>
@@ -55,6 +63,63 @@
     <t>Product Image File</t>
   </si>
   <si>
+    <t>#111</t>
+  </si>
+  <si>
+    <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit, sed do eiusmod tempor incididunt ut labore et dolore magna aliqua. Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut aliquip ex ea commodo consequat. Duis aute irure dolor in reprehenderit in voluptate velit esse cillum dolore eu fugiat nulla pariatur. Excepteur sint occaecat cupidatat non proident, sunt in culpa qui officia deserunt mollit anim id est laborum."</t>
+  </si>
+  <si>
+    <t>Sample Blah blah blah</t>
+  </si>
+  <si>
+    <t>New</t>
+  </si>
+  <si>
+    <t>Iphone</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>#222</t>
+  </si>
+  <si>
+    <t>Electronics &amp; Gadgets</t>
+  </si>
+  <si>
+    <t>Sahara</t>
+  </si>
+  <si>
+    <t>partner1</t>
+  </si>
+  <si>
+    <t>Style</t>
+  </si>
+  <si>
+    <t>Slug</t>
+  </si>
+  <si>
+    <t>sample1</t>
+  </si>
+  <si>
+    <t>1.png</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Luzon</t>
+  </si>
+  <si>
+    <t>Visayas</t>
+  </si>
+  <si>
+    <t>Mindanao</t>
+  </si>
+  <si>
+    <t>NCR</t>
+  </si>
+  <si>
     <t>Option name</t>
   </si>
   <si>
@@ -64,64 +129,19 @@
     <t>Option Price</t>
   </si>
   <si>
-    <t>#111</t>
-  </si>
-  <si>
-    <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit, sed do eiusmod tempor incididunt ut labore et dolore magna aliqua. Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut aliquip ex ea commodo consequat. Duis aute irure dolor in reprehenderit in voluptate velit esse cillum dolore eu fugiat nulla pariatur. Excepteur sint occaecat cupidatat non proident, sunt in culpa qui officia deserunt mollit anim id est laborum."</t>
-  </si>
-  <si>
-    <t>Sample Blah blah blah</t>
-  </si>
-  <si>
-    <t>New</t>
-  </si>
-  <si>
-    <t>Iphone</t>
-  </si>
-  <si>
-    <t>Color</t>
-  </si>
-  <si>
     <t>Red</t>
   </si>
   <si>
-    <t>#222</t>
-  </si>
-  <si>
-    <t>Electronics &amp; Gadgets</t>
-  </si>
-  <si>
-    <t>Jewellery &amp; Watches</t>
-  </si>
-  <si>
-    <t>Sahara</t>
-  </si>
-  <si>
-    <t>Sanrio</t>
-  </si>
-  <si>
-    <t>partner1</t>
-  </si>
-  <si>
-    <t>partner2</t>
-  </si>
-  <si>
-    <t>Style</t>
-  </si>
-  <si>
-    <t>Slug</t>
-  </si>
-  <si>
-    <t>sample1</t>
-  </si>
-  <si>
-    <t>sample2</t>
-  </si>
-  <si>
-    <t>2.jpg</t>
-  </si>
-  <si>
-    <t>1.png</t>
+    <t>Product Number</t>
+  </si>
+  <si>
+    <t>Orange</t>
+  </si>
+  <si>
+    <t>Shipping Location</t>
+  </si>
+  <si>
+    <t>Shipping Price</t>
   </si>
 </sst>
 </file>
@@ -454,10 +474,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:R3"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1:S3"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -468,16 +488,18 @@
     <col min="4" max="5" width="11.5703125"/>
     <col min="6" max="6" width="7.28515625"/>
     <col min="7" max="7" width="17.140625"/>
-    <col min="8" max="8" width="11.5703125"/>
+    <col min="8" max="8" width="11.5703125" customWidth="1"/>
     <col min="10" max="11" width="11.5703125"/>
     <col min="12" max="12" width="16.42578125"/>
     <col min="14" max="14" width="17.85546875"/>
     <col min="15" max="15" width="18.140625"/>
     <col min="16" max="16" width="14.85546875"/>
-    <col min="17" max="1027" width="11.5703125"/>
+    <col min="17" max="19" width="11.5703125"/>
+    <col min="20" max="21" width="16.5703125" customWidth="1"/>
+    <col min="22" max="1027" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:16">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -503,7 +525,7 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="J1" t="s">
         <v>8</v>
@@ -515,7 +537,7 @@
         <v>10</v>
       </c>
       <c r="M1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="N1" t="s">
         <v>11</v>
@@ -524,125 +546,57 @@
         <v>12</v>
       </c>
       <c r="P1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2" t="s">
         <v>13</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>14</v>
-      </c>
-      <c r="R1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18">
-      <c r="A2" t="s">
-        <v>16</v>
       </c>
       <c r="B2">
         <v>11111</v>
       </c>
       <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
         <v>17</v>
-      </c>
-      <c r="D2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" t="s">
-        <v>20</v>
       </c>
       <c r="G2">
         <v>32000</v>
       </c>
       <c r="H2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="I2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="J2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="L2">
         <v>12</v>
       </c>
       <c r="M2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="N2">
         <v>1</v>
       </c>
       <c r="O2" t="s">
-        <v>35</v>
-      </c>
-      <c r="P2" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>22</v>
-      </c>
-      <c r="R2">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18">
-      <c r="A3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3">
-        <v>22222</v>
-      </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3">
-        <v>32000</v>
-      </c>
-      <c r="H3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3" t="s">
-        <v>30</v>
-      </c>
-      <c r="J3" t="s">
-        <v>27</v>
-      </c>
-      <c r="K3" t="s">
-        <v>29</v>
-      </c>
-      <c r="L3">
+        <v>26</v>
+      </c>
+      <c r="P2">
         <v>12</v>
-      </c>
-      <c r="M3" t="s">
-        <v>33</v>
-      </c>
-      <c r="N3">
-        <v>1</v>
-      </c>
-      <c r="O3" t="s">
-        <v>34</v>
-      </c>
-      <c r="P3" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>22</v>
-      </c>
-      <c r="R3">
-        <v>1200</v>
       </c>
     </row>
   </sheetData>
@@ -653,4 +607,158 @@
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="16.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3">
+        <v>333</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A11:A1048576">
+      <formula1>locations</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="16.140625" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2">
+        <v>111</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:A1048576 B2:B1048576">
+      <formula1>locations</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="2" max="2" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
#159 changed csv_upload format
</commit_message>
<xml_diff>
--- a/public/misc/CSV_Upload.xlsx
+++ b/public/misc/CSV_Upload.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="473" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="473" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Products" sheetId="1" r:id="rId1"/>
     <sheet name="Attributes" sheetId="2" r:id="rId2"/>
     <sheet name="Shipment" sheetId="8" r:id="rId3"/>
     <sheet name="Locations" sheetId="7" r:id="rId4"/>
+    <sheet name="Images" sheetId="9" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="location">#REF!,#REF!,#REF!,#REF!,#REF!</definedName>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="49">
   <si>
     <t>Number</t>
   </si>
@@ -87,12 +88,21 @@
     <t>Electronics &amp; Gadgets</t>
   </si>
   <si>
+    <t>Jewellery &amp; Watches</t>
+  </si>
+  <si>
     <t>Sahara</t>
   </si>
   <si>
+    <t>Sanrio</t>
+  </si>
+  <si>
     <t>partner1</t>
   </si>
   <si>
+    <t>partner2</t>
+  </si>
+  <si>
     <t>Style</t>
   </si>
   <si>
@@ -102,6 +112,12 @@
     <t>sample1</t>
   </si>
   <si>
+    <t>sample2</t>
+  </si>
+  <si>
+    <t>2.jpg</t>
+  </si>
+  <si>
     <t>1.png</t>
   </si>
   <si>
@@ -138,10 +154,22 @@
     <t>Orange</t>
   </si>
   <si>
+    <t>Indigo</t>
+  </si>
+  <si>
     <t>Shipping Location</t>
   </si>
   <si>
     <t>Shipping Price</t>
+  </si>
+  <si>
+    <t>Size</t>
+  </si>
+  <si>
+    <t>Small</t>
+  </si>
+  <si>
+    <t>Option Image</t>
   </si>
 </sst>
 </file>
@@ -474,10 +502,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -525,7 +553,7 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="J1" t="s">
         <v>8</v>
@@ -537,7 +565,7 @@
         <v>10</v>
       </c>
       <c r="M1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="N1" t="s">
         <v>11</v>
@@ -546,7 +574,7 @@
         <v>12</v>
       </c>
       <c r="P1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:16">
@@ -575,28 +603,78 @@
         <v>20</v>
       </c>
       <c r="I2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="J2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L2">
         <v>12</v>
       </c>
       <c r="M2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="N2">
         <v>1</v>
       </c>
       <c r="O2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="P2">
         <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3">
+        <v>22222</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3">
+        <v>32000</v>
+      </c>
+      <c r="H3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" t="s">
+        <v>25</v>
+      </c>
+      <c r="L3">
+        <v>12</v>
+      </c>
+      <c r="M3" t="s">
+        <v>29</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3" t="s">
+        <v>30</v>
+      </c>
+      <c r="P3">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -611,10 +689,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -623,23 +701,27 @@
     <col min="2" max="2" width="12.85546875" customWidth="1"/>
     <col min="3" max="3" width="13.42578125" customWidth="1"/>
     <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+        <v>39</v>
+      </c>
+      <c r="E1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -647,29 +729,57 @@
         <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D2">
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
         <v>19</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>18</v>
       </c>
-      <c r="C3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3">
+      <c r="C4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4">
         <v>333</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5">
+        <v>444</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A11:A1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6:A1048576">
       <formula1>locations</formula1>
     </dataValidation>
   </dataValidations>
@@ -680,10 +790,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -695,13 +805,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B1" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="C1" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -709,15 +819,37 @@
         <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="C2">
         <v>111</v>
       </c>
     </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3">
+        <v>3333</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4">
+        <v>444</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:A1048576 B2:B1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:A1048576 B2:B1048576">
       <formula1>locations</formula1>
     </dataValidation>
   </dataValidations>
@@ -740,25 +872,96 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="2" width="16.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:A1048576">
+      <formula1>locations</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
#changed column format for product number
</commit_message>
<xml_diff>
--- a/public/misc/CSV_Upload.xlsx
+++ b/public/misc/CSV_Upload.xlsx
@@ -788,14 +788,12 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="16.140625" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" customWidth="1"/>
+    <col min="1" max="3" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -844,7 +842,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:A1048576 B2:B1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576">
       <formula1>locations</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
#435 removed slug column
</commit_message>
<xml_diff>
--- a/public/misc/CSV_Upload.xlsx
+++ b/public/misc/CSV_Upload.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="473" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="473"/>
   </bookViews>
   <sheets>
     <sheet name="Products" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="51">
   <si>
     <t>Number</t>
   </si>
@@ -94,9 +94,6 @@
     <t>Style</t>
   </si>
   <si>
-    <t>Slug</t>
-  </si>
-  <si>
     <t>2.jpg</t>
   </si>
   <si>
@@ -179,9 +176,6 @@
   </si>
   <si>
     <t>ccc.jpg</t>
-  </si>
-  <si>
-    <t>Cherry Mobile</t>
   </si>
 </sst>
 </file>
@@ -514,10 +508,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -531,15 +525,15 @@
     <col min="8" max="8" width="11.5703125" customWidth="1"/>
     <col min="10" max="11" width="11.5703125"/>
     <col min="12" max="12" width="16.42578125"/>
-    <col min="14" max="14" width="17.85546875"/>
-    <col min="15" max="15" width="18.140625"/>
-    <col min="16" max="16" width="14.85546875"/>
-    <col min="17" max="19" width="11.5703125"/>
-    <col min="20" max="21" width="16.5703125" customWidth="1"/>
-    <col min="22" max="1027" width="11.5703125"/>
+    <col min="13" max="13" width="17.85546875"/>
+    <col min="14" max="14" width="18.140625"/>
+    <col min="15" max="15" width="14.85546875"/>
+    <col min="16" max="18" width="11.5703125"/>
+    <col min="19" max="20" width="16.5703125" customWidth="1"/>
+    <col min="21" max="1026" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -577,19 +571,16 @@
         <v>10</v>
       </c>
       <c r="M1" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="N1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="O1" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -618,28 +609,25 @@
         <v>22</v>
       </c>
       <c r="J2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L2">
         <v>12</v>
       </c>
-      <c r="M2" t="s">
-        <v>52</v>
-      </c>
-      <c r="N2">
+      <c r="M2">
         <v>1</v>
       </c>
-      <c r="O2" t="s">
-        <v>44</v>
-      </c>
-      <c r="P2">
+      <c r="N2" t="s">
+        <v>43</v>
+      </c>
+      <c r="O2">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:15">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -668,24 +656,21 @@
         <v>22</v>
       </c>
       <c r="J3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L3">
         <v>12</v>
       </c>
-      <c r="M3" t="s">
-        <v>52</v>
-      </c>
-      <c r="N3">
+      <c r="M3">
         <v>1</v>
       </c>
-      <c r="O3" t="s">
-        <v>24</v>
-      </c>
-      <c r="P3">
+      <c r="N3" t="s">
+        <v>23</v>
+      </c>
+      <c r="O3">
         <v>13</v>
       </c>
     </row>
@@ -717,19 +702,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
         <v>30</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>31</v>
       </c>
-      <c r="D1" t="s">
-        <v>32</v>
-      </c>
       <c r="E1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -740,13 +725,13 @@
         <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D2">
         <v>111</v>
       </c>
       <c r="E2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -757,13 +742,13 @@
         <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D3">
         <v>21342</v>
       </c>
       <c r="E3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -771,16 +756,16 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" t="s">
         <v>38</v>
-      </c>
-      <c r="C4" t="s">
-        <v>39</v>
       </c>
       <c r="D4">
         <v>222</v>
       </c>
       <c r="E4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -791,13 +776,13 @@
         <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D5">
         <v>333</v>
       </c>
       <c r="E5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -805,16 +790,16 @@
         <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D6">
         <v>444</v>
       </c>
       <c r="E6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -822,16 +807,16 @@
         <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D7">
         <v>444</v>
       </c>
       <c r="E7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -857,13 +842,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s">
         <v>36</v>
-      </c>
-      <c r="C1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -871,7 +856,7 @@
         <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C2">
         <v>111</v>
@@ -882,7 +867,7 @@
         <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C3">
         <v>3333</v>
@@ -893,7 +878,7 @@
         <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C4">
         <v>444</v>
@@ -924,22 +909,22 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -951,7 +936,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -962,7 +947,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
         <v>12</v>
@@ -973,7 +958,7 @@
         <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -981,7 +966,7 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -989,7 +974,7 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -997,7 +982,7 @@
         <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1005,7 +990,7 @@
         <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1013,7 +998,7 @@
         <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#439 removed uncessary style column
</commit_message>
<xml_diff>
--- a/public/misc/CSV_Upload.xlsx
+++ b/public/misc/CSV_Upload.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="473" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="473"/>
   </bookViews>
   <sheets>
     <sheet name="Products" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="52">
   <si>
     <t>Number</t>
   </si>
@@ -89,9 +89,6 @@
   </si>
   <si>
     <t>Jewellery &amp; Watches</t>
-  </si>
-  <si>
-    <t>Style</t>
   </si>
   <si>
     <t>Slug</t>
@@ -514,10 +511,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -529,17 +526,17 @@
     <col min="6" max="6" width="7.28515625"/>
     <col min="7" max="7" width="17.140625"/>
     <col min="8" max="8" width="11.5703125" customWidth="1"/>
-    <col min="10" max="11" width="11.5703125"/>
-    <col min="12" max="12" width="16.42578125"/>
-    <col min="14" max="14" width="17.85546875"/>
-    <col min="15" max="15" width="18.140625"/>
-    <col min="16" max="16" width="14.85546875"/>
-    <col min="17" max="19" width="11.5703125"/>
-    <col min="20" max="21" width="16.5703125" customWidth="1"/>
-    <col min="22" max="1027" width="11.5703125"/>
+    <col min="9" max="10" width="11.5703125"/>
+    <col min="11" max="11" width="16.42578125"/>
+    <col min="13" max="13" width="17.85546875"/>
+    <col min="14" max="14" width="18.140625"/>
+    <col min="15" max="15" width="14.85546875"/>
+    <col min="16" max="18" width="11.5703125"/>
+    <col min="19" max="20" width="16.5703125" customWidth="1"/>
+    <col min="21" max="1026" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -565,31 +562,28 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
         <v>22</v>
       </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" t="s">
-        <v>10</v>
-      </c>
       <c r="M1" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="N1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="O1" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -615,31 +609,28 @@
         <v>20</v>
       </c>
       <c r="I2" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="J2" t="s">
-        <v>42</v>
-      </c>
-      <c r="K2" t="s">
-        <v>41</v>
-      </c>
-      <c r="L2">
+        <v>40</v>
+      </c>
+      <c r="K2">
         <v>12</v>
       </c>
-      <c r="M2" t="s">
-        <v>52</v>
-      </c>
-      <c r="N2">
+      <c r="L2" t="s">
+        <v>51</v>
+      </c>
+      <c r="M2">
         <v>1</v>
       </c>
-      <c r="O2" t="s">
-        <v>44</v>
-      </c>
-      <c r="P2">
+      <c r="N2" t="s">
+        <v>43</v>
+      </c>
+      <c r="O2">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:15">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -665,27 +656,24 @@
         <v>21</v>
       </c>
       <c r="I3" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="J3" t="s">
-        <v>43</v>
-      </c>
-      <c r="K3" t="s">
-        <v>41</v>
-      </c>
-      <c r="L3">
+        <v>40</v>
+      </c>
+      <c r="K3">
         <v>12</v>
       </c>
-      <c r="M3" t="s">
-        <v>52</v>
-      </c>
-      <c r="N3">
+      <c r="L3" t="s">
+        <v>51</v>
+      </c>
+      <c r="M3">
         <v>1</v>
       </c>
-      <c r="O3" t="s">
-        <v>24</v>
-      </c>
-      <c r="P3">
+      <c r="N3" t="s">
+        <v>23</v>
+      </c>
+      <c r="O3">
         <v>13</v>
       </c>
     </row>
@@ -717,19 +705,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
         <v>30</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>31</v>
       </c>
-      <c r="D1" t="s">
-        <v>32</v>
-      </c>
       <c r="E1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -740,13 +728,13 @@
         <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D2">
         <v>111</v>
       </c>
       <c r="E2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -757,13 +745,13 @@
         <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D3">
         <v>21342</v>
       </c>
       <c r="E3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -771,16 +759,16 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" t="s">
         <v>38</v>
-      </c>
-      <c r="C4" t="s">
-        <v>39</v>
       </c>
       <c r="D4">
         <v>222</v>
       </c>
       <c r="E4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -791,13 +779,13 @@
         <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D5">
         <v>333</v>
       </c>
       <c r="E5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -805,16 +793,16 @@
         <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D6">
         <v>444</v>
       </c>
       <c r="E6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -822,16 +810,16 @@
         <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D7">
         <v>444</v>
       </c>
       <c r="E7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -857,13 +845,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s">
         <v>36</v>
-      </c>
-      <c r="C1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -871,7 +859,7 @@
         <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C2">
         <v>111</v>
@@ -882,7 +870,7 @@
         <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C3">
         <v>3333</v>
@@ -893,7 +881,7 @@
         <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C4">
         <v>444</v>
@@ -924,22 +912,22 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -951,7 +939,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -962,7 +950,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
         <v>12</v>
@@ -973,7 +961,7 @@
         <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -981,7 +969,7 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -989,7 +977,7 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -997,7 +985,7 @@
         <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1005,7 +993,7 @@
         <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1013,7 +1001,7 @@
         <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#439 removed slug because auto-merge failed
</commit_message>
<xml_diff>
--- a/public/misc/CSV_Upload.xlsx
+++ b/public/misc/CSV_Upload.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="50">
   <si>
     <t>Number</t>
   </si>
@@ -91,9 +91,6 @@
     <t>Jewellery &amp; Watches</t>
   </si>
   <si>
-    <t>Slug</t>
-  </si>
-  <si>
     <t>2.jpg</t>
   </si>
   <si>
@@ -176,9 +173,6 @@
   </si>
   <si>
     <t>ccc.jpg</t>
-  </si>
-  <si>
-    <t>Cherry Mobile</t>
   </si>
 </sst>
 </file>
@@ -511,10 +505,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -528,15 +522,15 @@
     <col min="8" max="8" width="11.5703125" customWidth="1"/>
     <col min="9" max="10" width="11.5703125"/>
     <col min="11" max="11" width="16.42578125"/>
-    <col min="13" max="13" width="17.85546875"/>
-    <col min="14" max="14" width="18.140625"/>
-    <col min="15" max="15" width="14.85546875"/>
-    <col min="16" max="18" width="11.5703125"/>
-    <col min="19" max="20" width="16.5703125" customWidth="1"/>
-    <col min="21" max="1026" width="11.5703125"/>
+    <col min="12" max="12" width="17.85546875"/>
+    <col min="13" max="13" width="18.140625"/>
+    <col min="14" max="14" width="14.85546875"/>
+    <col min="15" max="17" width="11.5703125"/>
+    <col min="18" max="19" width="16.5703125" customWidth="1"/>
+    <col min="20" max="1025" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -571,19 +565,16 @@
         <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="M1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -609,28 +600,25 @@
         <v>20</v>
       </c>
       <c r="I2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K2">
         <v>12</v>
       </c>
-      <c r="L2" t="s">
-        <v>51</v>
-      </c>
-      <c r="M2">
+      <c r="L2">
         <v>1</v>
       </c>
-      <c r="N2" t="s">
-        <v>43</v>
-      </c>
-      <c r="O2">
+      <c r="M2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N2">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:14">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -656,24 +644,21 @@
         <v>21</v>
       </c>
       <c r="I3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K3">
         <v>12</v>
       </c>
-      <c r="L3" t="s">
-        <v>51</v>
-      </c>
-      <c r="M3">
+      <c r="L3">
         <v>1</v>
       </c>
-      <c r="N3" t="s">
-        <v>23</v>
-      </c>
-      <c r="O3">
+      <c r="M3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N3">
         <v>13</v>
       </c>
     </row>
@@ -705,19 +690,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
         <v>29</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>30</v>
       </c>
-      <c r="D1" t="s">
-        <v>31</v>
-      </c>
       <c r="E1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -728,13 +713,13 @@
         <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D2">
         <v>111</v>
       </c>
       <c r="E2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -745,13 +730,13 @@
         <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D3">
         <v>21342</v>
       </c>
       <c r="E3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -759,16 +744,16 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" t="s">
         <v>37</v>
-      </c>
-      <c r="C4" t="s">
-        <v>38</v>
       </c>
       <c r="D4">
         <v>222</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -779,13 +764,13 @@
         <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D5">
         <v>333</v>
       </c>
       <c r="E5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -793,16 +778,16 @@
         <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D6">
         <v>444</v>
       </c>
       <c r="E6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -810,16 +795,16 @@
         <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D7">
         <v>444</v>
       </c>
       <c r="E7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -845,13 +830,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" t="s">
         <v>35</v>
-      </c>
-      <c r="C1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -859,7 +844,7 @@
         <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C2">
         <v>111</v>
@@ -870,7 +855,7 @@
         <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3">
         <v>3333</v>
@@ -881,7 +866,7 @@
         <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C4">
         <v>444</v>
@@ -912,22 +897,22 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -950,7 +935,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B1" t="s">
         <v>12</v>
@@ -961,7 +946,7 @@
         <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -969,7 +954,7 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -977,7 +962,7 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -985,7 +970,7 @@
         <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -993,7 +978,7 @@
         <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1001,7 +986,7 @@
         <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#439 changed column format
</commit_message>
<xml_diff>
--- a/public/misc/CSV_Upload.xlsx
+++ b/public/misc/CSV_Upload.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="473"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="473" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Products" sheetId="1" r:id="rId1"/>
@@ -507,8 +507,8 @@
   </sheetPr>
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -677,7 +677,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -818,12 +818,11 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="16.140625" customWidth="1"/>
     <col min="2" max="2" width="17.28515625" customWidth="1"/>
     <col min="3" max="3" width="12.85546875" customWidth="1"/>
   </cols>
@@ -874,7 +873,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:A1048576 B2:B1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576">
       <formula1>locations</formula1>
     </dataValidation>
   </dataValidations>
@@ -887,7 +886,7 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -924,8 +923,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>

</xml_diff>

<commit_message>
#441 Added style column
</commit_message>
<xml_diff>
--- a/public/misc/CSV_Upload.xlsx
+++ b/public/misc/CSV_Upload.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="473" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="473"/>
   </bookViews>
   <sheets>
     <sheet name="Products" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="51">
   <si>
     <t>Number</t>
   </si>
@@ -173,6 +173,9 @@
   </si>
   <si>
     <t>ccc.jpg</t>
+  </si>
+  <si>
+    <t>Style</t>
   </si>
 </sst>
 </file>
@@ -505,10 +508,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -520,17 +523,18 @@
     <col min="6" max="6" width="7.28515625"/>
     <col min="7" max="7" width="17.140625"/>
     <col min="8" max="8" width="11.5703125" customWidth="1"/>
-    <col min="9" max="10" width="11.5703125"/>
-    <col min="11" max="11" width="16.42578125"/>
-    <col min="12" max="12" width="17.85546875"/>
-    <col min="13" max="13" width="18.140625"/>
-    <col min="14" max="14" width="14.85546875"/>
-    <col min="15" max="17" width="11.5703125"/>
-    <col min="18" max="19" width="16.5703125" customWidth="1"/>
-    <col min="20" max="1025" width="11.5703125"/>
+    <col min="9" max="9" width="11.5703125"/>
+    <col min="11" max="11" width="11.5703125"/>
+    <col min="12" max="12" width="16.42578125"/>
+    <col min="13" max="13" width="17.85546875"/>
+    <col min="14" max="14" width="18.140625"/>
+    <col min="15" max="15" width="14.85546875"/>
+    <col min="16" max="18" width="11.5703125"/>
+    <col min="19" max="20" width="16.5703125" customWidth="1"/>
+    <col min="21" max="1026" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -559,22 +563,25 @@
         <v>8</v>
       </c>
       <c r="J1" t="s">
+        <v>50</v>
+      </c>
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -602,23 +609,26 @@
       <c r="I2" t="s">
         <v>40</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
         <v>39</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>12</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>1</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>42</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:15">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -646,19 +656,22 @@
       <c r="I3" t="s">
         <v>41</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3" t="s">
         <v>39</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>12</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>1</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>22</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>13</v>
       </c>
     </row>
@@ -923,7 +936,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
#441 made use of constant value for style column
</commit_message>
<xml_diff>
--- a/public/misc/CSV_Upload.xlsx
+++ b/public/misc/CSV_Upload.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="50">
   <si>
     <t>Number</t>
   </si>
@@ -173,9 +173,6 @@
   </si>
   <si>
     <t>ccc.jpg</t>
-  </si>
-  <si>
-    <t>Style</t>
   </si>
 </sst>
 </file>
@@ -508,10 +505,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -523,18 +520,17 @@
     <col min="6" max="6" width="7.28515625"/>
     <col min="7" max="7" width="17.140625"/>
     <col min="8" max="8" width="11.5703125" customWidth="1"/>
-    <col min="9" max="9" width="11.5703125"/>
-    <col min="11" max="11" width="11.5703125"/>
-    <col min="12" max="12" width="16.42578125"/>
-    <col min="13" max="13" width="17.85546875"/>
-    <col min="14" max="14" width="18.140625"/>
-    <col min="15" max="15" width="14.85546875"/>
-    <col min="16" max="18" width="11.5703125"/>
-    <col min="19" max="20" width="16.5703125" customWidth="1"/>
-    <col min="21" max="1026" width="11.5703125"/>
+    <col min="9" max="10" width="11.5703125"/>
+    <col min="11" max="11" width="16.42578125"/>
+    <col min="12" max="12" width="17.85546875"/>
+    <col min="13" max="13" width="18.140625"/>
+    <col min="14" max="14" width="14.85546875"/>
+    <col min="15" max="17" width="11.5703125"/>
+    <col min="18" max="19" width="16.5703125" customWidth="1"/>
+    <col min="20" max="1025" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -563,25 +559,22 @@
         <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>50</v>
+        <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -609,26 +602,23 @@
       <c r="I2" t="s">
         <v>40</v>
       </c>
-      <c r="J2">
+      <c r="J2" t="s">
+        <v>39</v>
+      </c>
+      <c r="K2">
+        <v>12</v>
+      </c>
+      <c r="L2">
         <v>1</v>
       </c>
-      <c r="K2" t="s">
-        <v>39</v>
-      </c>
-      <c r="L2">
+      <c r="M2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N2">
         <v>12</v>
       </c>
-      <c r="M2">
-        <v>1</v>
-      </c>
-      <c r="N2" t="s">
-        <v>42</v>
-      </c>
-      <c r="O2">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15">
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -656,22 +646,19 @@
       <c r="I3" t="s">
         <v>41</v>
       </c>
-      <c r="J3">
+      <c r="J3" t="s">
+        <v>39</v>
+      </c>
+      <c r="K3">
+        <v>12</v>
+      </c>
+      <c r="L3">
         <v>1</v>
       </c>
-      <c r="K3" t="s">
-        <v>39</v>
-      </c>
-      <c r="L3">
-        <v>12</v>
-      </c>
-      <c r="M3">
-        <v>1</v>
-      </c>
-      <c r="N3" t="s">
+      <c r="M3" t="s">
         <v>22</v>
       </c>
-      <c r="O3">
+      <c r="N3">
         <v>13</v>
       </c>
     </row>

</xml_diff>